<commit_message>
'linear ok, log em desenvolvimento'
</commit_message>
<xml_diff>
--- a/Tabela_pib_per_capita_brasileiro.xlsx
+++ b/Tabela_pib_per_capita_brasileiro.xlsx
@@ -329,7 +329,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -614,11 +614,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="47432033"/>
-        <c:axId val="3505957"/>
+        <c:axId val="56461510"/>
+        <c:axId val="72343973"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47432033"/>
+        <c:axId val="56461510"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -646,12 +646,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3505957"/>
+        <c:crossAx val="72343973"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="3505957"/>
+        <c:axId val="72343973"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,7 +688,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47432033"/>
+        <c:crossAx val="56461510"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -736,7 +736,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1032,11 +1032,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="94632691"/>
-        <c:axId val="22129068"/>
+        <c:axId val="2890674"/>
+        <c:axId val="6384344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94632691"/>
+        <c:axId val="2890674"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,12 +1064,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22129068"/>
+        <c:crossAx val="6384344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="22129068"/>
+        <c:axId val="6384344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1106,7 +1106,1263 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94632691"/>
+        <c:crossAx val="2890674"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="pt-BR" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>exponencial</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.833125"/>
+          <c:y val="0.0831111111111111"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.127570473154572"/>
+          <c:y val="0.0328369818868763"/>
+          <c:w val="0.682667666729171"/>
+          <c:h val="0.865540615623958"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="ff0000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Tabela!$A$2:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabela!$B$2:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>5219.36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5729.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5944.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6359.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6900.62</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7467.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8340.58</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9506.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10705.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11733.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12880.52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14390.01</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16280.82</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17271.34</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19938.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>22259.91</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24278.35</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26657.54</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28648.74</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>29466.85</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30558.75</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31843.95</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>33593.82</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>35161.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>35935.69</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="64893007"/>
+        <c:axId val="10309070"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="64893007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="10309070"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="10309070"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64893007"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.82192637039815"/>
+          <c:y val="0.439159906656295"/>
+          <c:w val="0.164947809238077"/>
+          <c:h val="0.12168018668741"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="pt-BR" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Geométrico</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.8334375"/>
+          <c:y val="0.0741111111111111"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0935370960685043"/>
+          <c:y val="0.00605622846982995"/>
+          <c:w val="0.739983748984312"/>
+          <c:h val="0.865985109456606"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="ff0000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Tabela!$A$2:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabela!$B$2:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>5219.36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5729.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5944.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6359.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6900.62</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7467.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8340.58</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9506.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10705.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11733.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12880.52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14390.01</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16280.82</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17271.34</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19938.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>22259.91</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24278.35</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26657.54</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28648.74</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>29466.85</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30558.75</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31843.95</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>33593.82</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>35161.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>35935.69</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="94486725"/>
+        <c:axId val="53331584"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="94486725"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="53331584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="53331584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="94486725"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="pt-BR" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Polinomial de grau 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabela!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PIB per capita-valores correntes (Reais)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="ff0000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Tabela!$A$2:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabela!$B$2:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>5219.36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5729.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5944.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6359.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6900.62</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7467.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8340.58</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9506.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10705.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11733.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12880.52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14390.01</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16280.82</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17271.34</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19938.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>22259.91</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24278.35</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26657.54</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28648.74</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>29466.85</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30558.75</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31843.95</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>33593.82</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>35161.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>35935.69</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="10681026"/>
+        <c:axId val="24571564"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="10681026"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="24571564"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="24571564"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="10681026"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1216,6 +2472,96 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>233280</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>104400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>676440</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>14040</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="3270960" y="7465320"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>332280</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>94680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>16200</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>4680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="3369960" y="11136240"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>460800</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>16560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>144720</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>101520</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="3498480" y="14913720"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1226,8 +2572,8 @@
   </sheetPr>
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O94" activeCellId="0" sqref="O94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>